<commit_message>
Ajout dans dossiers filaires triangles
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mik75\Documents\S8-PLMmaquettage\02 - Exemple_Maquette\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75692EB4-CB03-4D9D-A66E-74F304BDF0CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E0D858-3C12-4A6C-AD66-F3A5CA54E804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1185" windowWidth="17805" windowHeight="11505" xr2:uid="{C1D3470F-B8EA-47E3-BA2C-3E90D6507FF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C1D3470F-B8EA-47E3-BA2C-3E90D6507FF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,16 +416,16 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,15 +433,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -449,7 +449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -457,7 +457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -465,7 +465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -473,7 +473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -481,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -489,7 +489,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Mise en place Suspension sur la maquette
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E0D858-3C12-4A6C-AD66-F3A5CA54E804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE6590D-EC2C-431E-849F-3F22E944819B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C1D3470F-B8EA-47E3-BA2C-3E90D6507FF5}"/>
+    <workbookView xWindow="9636" yWindow="492" windowWidth="11268" windowHeight="11868" xr2:uid="{C1D3470F-B8EA-47E3-BA2C-3E90D6507FF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>entretoise_upright (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_rotule (mm)</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497D7EFB-D4A5-49A2-922B-BCB3E28C5B81}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,6 +500,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Design table pour inserts
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -5,35 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE6590D-EC2C-431E-849F-3F22E944819B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2964AB0E-FEE3-4B95-9A98-E75A55AD858E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9636" yWindow="492" windowWidth="11268" windowHeight="11868" xr2:uid="{C1D3470F-B8EA-47E3-BA2C-3E90D6507FF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -63,6 +64,18 @@
   </si>
   <si>
     <t>Rayon_rotule (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_collage_plug (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_rotule (mm)</t>
+  </si>
+  <si>
+    <t>Plug_rint (mm)</t>
+  </si>
+  <si>
+    <t>Plug_rext (mm)</t>
   </si>
 </sst>
 </file>
@@ -72,10 +85,10 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,7 +133,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -415,14 +428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497D7EFB-D4A5-49A2-922B-BCB3E28C5B81}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
@@ -505,10 +518,44 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B11" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <f>15.7/2</f>
+        <v>7.85</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
attaches pullrod sur inserts
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2964AB0E-FEE3-4B95-9A98-E75A55AD858E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC46DD5-53BD-4CCB-967B-085DDE65875F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>Plug_rext (mm)</t>
+  </si>
+  <si>
+    <t>Espacement_attaches_pullrod (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_attaches_pullrod (mm)</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,6 +560,22 @@
         <v>7.85</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Modification catia front rocker
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB07F4A6-354D-479A-A949-50491B414DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE491D09-C7F5-4012-8D12-58A5511A5DDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Rayon_attaches_pullrod (mm)</t>
+  </si>
+  <si>
+    <t>Half_Rocker_Width (mm)</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,13 +438,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
@@ -576,6 +579,14 @@
         <v>3.2</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Mise en place suspension rod
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE491D09-C7F5-4012-8D12-58A5511A5DDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109A80FF-7BED-4942-AD37-A559B5B22188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="816" yWindow="744" windowWidth="15072" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>Half_Rocker_Width (mm)</t>
+  </si>
+  <si>
+    <t>Pull_rod_Offset (mm)</t>
+  </si>
+  <si>
+    <t>Push_rod_Offset (mm)</t>
+  </si>
+  <si>
+    <t>Suspension_Rod_Rint (mm)</t>
+  </si>
+  <si>
+    <t>Suspension_Rod_Rext (mm)</t>
   </si>
 </sst>
 </file>
@@ -438,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +599,38 @@
         <v>7.5</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Ajustement offset RU + nettoyage SU_01003
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B44A54-AC42-406A-A869-A1321594381A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA072ADD-4BF4-4A2E-A371-5626F1D26EAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -453,7 +453,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
push BAR + modif params
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthieu\Documents\EPSA\GIT\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032FCFEB-EF3F-4F35-BB20-E5C1615DABDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E3BDAA-9BD1-4738-B58A-2D2986698F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>rayon_vis_basculeurs_autres (mm)</t>
+  </si>
+  <si>
+    <t>debut_porte_couteaux (mm)</t>
   </si>
 </sst>
 </file>
@@ -169,7 +172,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -465,19 +468,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +488,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -493,7 +496,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -501,7 +504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -509,7 +512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -517,7 +520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,7 +528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -533,7 +536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -541,7 +544,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -549,7 +552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -557,7 +560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -565,7 +568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -573,7 +576,7 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -581,7 +584,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -590,7 +593,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -598,7 +601,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -606,7 +609,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -614,7 +617,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -622,7 +625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -630,7 +633,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -638,7 +641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -646,7 +649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -654,7 +657,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -662,7 +665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -670,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -678,12 +681,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2">
         <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
params+porte couteaux + couteaux + barre
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthieu\Documents\EPSA\GIT\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E3BDAA-9BD1-4738-B58A-2D2986698F09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A253A950-FC6F-4F4E-8B93-10C59D3A6084}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>debut_porte_couteaux (mm)</t>
+  </si>
+  <si>
+    <t>debut_couteaux (mm)</t>
+  </si>
+  <si>
+    <t>r_int_BAR (mm)</t>
+  </si>
+  <si>
+    <t>r_ext_BAR (mm)</t>
+  </si>
+  <si>
+    <t>r_ini_couteaux (mm)</t>
   </si>
 </sst>
 </file>
@@ -468,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,6 +709,38 @@
         <v>10</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
SU Ajout Tie rod
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthieu\Documents\EPSA\GIT\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85BB68B-4D45-4574-9D80-5AEEFA1BFBA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6F413D-5953-48C2-9F55-EA6ABD80FFDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>r_ini_couteaux (mm)</t>
+  </si>
+  <si>
+    <t>TieRod_tubeOffset (mm)</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,6 +733,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
ajustement inserts nouvelles rotules
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6F413D-5953-48C2-9F55-EA6ABD80FFDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A204E27-2D4E-4136-876C-A825A5890A73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -483,10 +483,10 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
@@ -569,7 +569,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>8</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -585,7 +585,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>6.75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SU Maj tubes et cache contraintes
Maj rayon tubes -> comme l'an dernier
Caches contraintes dans divers assemblages et caches plan, repères et wire
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A204E27-2D4E-4136-876C-A825A5890A73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9665EA-7A9A-4789-BAA9-128CB095F7DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="900" windowWidth="17580" windowHeight="11436" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -483,10 +483,10 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
@@ -537,7 +537,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -545,7 +545,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -650,7 +650,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -658,7 +658,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>10</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SU debut assemblage Front Rocker
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\GIT\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB49900A-5D4A-454A-A595-3979A8650B9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA6A13C-C9CF-40E9-8AB4-CB174AB564D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>Suspension_Rod_Rint (mm)</t>
-  </si>
-  <si>
-    <t>Suspension_Rod_Rext (mm)</t>
   </si>
   <si>
     <t>Longueur_couteaux (mm)</t>
@@ -480,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -626,7 +623,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>7.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -658,7 +655,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>9.75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -666,7 +663,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>80</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -682,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -690,7 +687,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -706,7 +703,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -714,7 +711,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -722,7 +719,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -730,14 +727,6 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SU suite assemblage Front Rocker
mise en place des vis pour BAR, Triangle et Damper. Rectification : suppression des rondelles côté écrou Knut
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\GIT\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA6A13C-C9CF-40E9-8AB4-CB174AB564D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7AEE75-9AE3-4D59-AC03-F6F7ADBE2D51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,7 +480,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +671,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>4</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>3</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Réparation de la maquette en tout genre SU/ST/WT
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\GIT\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5608880C-332B-418D-8F5C-AB0E373DB117}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52BF571-85CF-4444-8433-8BB48D11ECB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1812" windowWidth="17580" windowHeight="11436" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>AArm_tubeOffset_FU (mm)</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>TieRod_tubeOffset (mm)</t>
+  </si>
+  <si>
+    <t>Suspension_Rod_Rext (mm)</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,47 +655,47 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2">
-        <v>80</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>4</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="2">
-        <v>4.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="2">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>15</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2">
         <v>15</v>
@@ -700,33 +703,41 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="2">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SU changement rotules triangles
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\EPSA\Github\Valkyriz\ELIZ-2021\SU_Suspension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52BF571-85CF-4444-8433-8BB48D11ECB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FA6EB4-F9FB-41C8-BFA8-EC7CCE63C4C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1812" windowWidth="17580" windowHeight="11436" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3252" yWindow="1968" windowWidth="15336" windowHeight="8016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -482,11 +482,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
@@ -569,7 +569,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>9.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SU Correction épaisseur inserts
</commit_message>
<xml_diff>
--- a/SU_Suspension/params.xlsx
+++ b/SU_Suspension/params.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\OneDrive\Documents\Git\ELIZ-2021\SU_Suspension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FA6EB4-F9FB-41C8-BFA8-EC7CCE63C4C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F92C1F0-4A4B-4CAF-AD1E-C69C428F85BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3252" yWindow="1968" windowWidth="15336" windowHeight="8016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,7 +585,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>9</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>